<commit_message>
Modified WBS  and updated Asset list
To include specific Wireframes
</commit_message>
<xml_diff>
--- a/WBS.xlsx
+++ b/WBS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pclures03\home\1khans16\Documents\GitHub\Mobile-Applications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pclures01\home\3coylj96\Documents\GitHub\Mobile-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,10 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.0" hidden="1">Sheet1!$D$17:$D$73</definedName>
-    <definedName name="_xlchart.1" hidden="1">Sheet1!$E$17:$E$73</definedName>
-    <definedName name="_xlchart.2" hidden="1">Sheet1!$D$4:$D$76</definedName>
-    <definedName name="_xlchart.3" hidden="1">Sheet1!$E$4:$E$76</definedName>
+    <definedName name="_xlchart.0" hidden="1">Sheet1!$D$4:$D$83</definedName>
+    <definedName name="_xlchart.1" hidden="1">Sheet1!$E$4:$E$83</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>Tasks</t>
   </si>
@@ -252,6 +250,24 @@
   </si>
   <si>
     <t>UML/Class diagrams</t>
+  </si>
+  <si>
+    <t>Title Menu</t>
+  </si>
+  <si>
+    <t>Settings Menu</t>
+  </si>
+  <si>
+    <t>In-game UI</t>
+  </si>
+  <si>
+    <t>In-game Settings</t>
+  </si>
+  <si>
+    <t>Overworld menu</t>
+  </si>
+  <si>
+    <t>Pause Menu</t>
   </si>
 </sst>
 </file>
@@ -330,10 +346,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.2</cx:f>
+        <cx:f>_xlchart.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.3</cx:f>
+        <cx:f>_xlchart.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -868,13 +884,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1198,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E79"/>
+  <dimension ref="B2:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,429 +1337,388 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
+      <c r="C12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
+      <c r="C17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
         <v>59</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
         <v>59</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
       </c>
       <c r="E31">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
         <v>59</v>
       </c>
       <c r="E32">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>19</v>
       </c>
-      <c r="D33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33">
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>22</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D44" t="s">
         <v>58</v>
       </c>
-      <c r="E37">
+      <c r="E44">
         <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" t="s">
-        <v>58</v>
-      </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E45">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E46">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>22</v>
+      <c r="C48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>23</v>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51">
-        <v>0.5</v>
+      <c r="B51" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D55" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55">
-        <v>4</v>
+      <c r="B55" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E56">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D59" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E59">
         <v>2</v>
@@ -1751,72 +1726,78 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D61" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E61">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>25</v>
+      <c r="C62" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D63" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>51</v>
-      </c>
-      <c r="D64" t="s">
-        <v>63</v>
-      </c>
-      <c r="E64">
-        <v>2</v>
+      <c r="B64" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>26</v>
+      <c r="C66" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D67" t="s">
         <v>63</v>
@@ -1826,49 +1807,49 @@
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>27</v>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>54</v>
-      </c>
-      <c r="D69" t="s">
-        <v>59</v>
-      </c>
-      <c r="E69">
-        <v>4</v>
+      <c r="B69" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="D70" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E70">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D71" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E71">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D72" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E72">
         <v>4</v>
@@ -1876,48 +1857,113 @@
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E74">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" t="s">
-        <v>59</v>
-      </c>
-      <c r="E75">
-        <v>4</v>
+      <c r="B75" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D76" t="s">
         <v>59</v>
       </c>
       <c r="E76">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>59</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" t="s">
+        <v>59</v>
+      </c>
+      <c r="E78">
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
+      </c>
+      <c r="E79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" t="s">
+        <v>59</v>
+      </c>
+      <c r="E81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" t="s">
+        <v>59</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83" t="s">
+        <v>59</v>
+      </c>
+      <c r="E83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>64</v>
       </c>
-      <c r="E79">
-        <f>SUM(E17:E78)</f>
+      <c r="E86">
+        <f>SUM(E24:E85)</f>
         <v>171.5</v>
       </c>
     </row>

</xml_diff>